<commit_message>
[BUG] Fix failing test
</commit_message>
<xml_diff>
--- a/api/v1/module/App/test/sampleapp/content/entity/FieldValidationSample.xlsx
+++ b/api/v1/module/App/test/sampleapp/content/entity/FieldValidationSample.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eox3.0\api\v1\module\App\test\sampleapp\content\entity\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6394D6EC-620D-4FED-A7ED-056B20D35C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28560" windowHeight="12855"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,12 +49,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Rajesh</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -100,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="194">
   <si>
     <t>Field Name</t>
   </si>
@@ -676,13 +682,19 @@
   </si>
   <si>
     <t>longtext</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>Tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,39 +743,38 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q1048576" totalsRowShown="0">
-  <autoFilter ref="A1:Q1048576">
-    <filterColumn colId="2"/>
-    <filterColumn colId="5"/>
-    <filterColumn colId="6"/>
-    <filterColumn colId="10"/>
-    <filterColumn colId="11"/>
-    <filterColumn colId="12"/>
-    <filterColumn colId="13"/>
-    <filterColumn colId="14"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q1048572" totalsRowShown="0">
+  <autoFilter ref="A1:Q1048572" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Field Name"/>
-    <tableColumn id="2" name="Field Label"/>
-    <tableColumn id="10" name="Parent Field Name"/>
-    <tableColumn id="3" name="Field Type"/>
-    <tableColumn id="4" name="Data Type"/>
-    <tableColumn id="12" name="Item Name"/>
-    <tableColumn id="13" name="Item Label"/>
-    <tableColumn id="5" name="Place Holder Text"/>
-    <tableColumn id="9" name="Default Value"/>
-    <tableColumn id="6" name="Required?"/>
-    <tableColumn id="15" name="Min "/>
-    <tableColumn id="14" name="Max "/>
-    <tableColumn id="11" name="Decimal Places"/>
-    <tableColumn id="16" name="Regex Pattern"/>
-    <tableColumn id="17" name="Format"/>
-    <tableColumn id="7" name="Error Message"/>
-    <tableColumn id="8" name="Input Mask"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Field Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Field Label"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Parent Field Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field Type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data Type"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Item Name"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Item Label"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Place Holder Text"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Default Value"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Required?"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Min "/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Max "/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Decimal Places"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Regex Pattern"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Format"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Error Message"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Input Mask"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -812,7 +823,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,9 +855,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -878,6 +907,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1053,15 +1100,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q1996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="3" width="28.28515625" customWidth="1"/>
@@ -1077,7 +1124,7 @@
     <col min="33" max="34" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1177,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1156,7 +1203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1182,7 +1229,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1202,7 +1249,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1222,7 +1269,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>34</v>
       </c>
@@ -1233,7 +1280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>57</v>
       </c>
@@ -1244,7 +1291,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>59</v>
       </c>
@@ -1258,7 +1305,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1278,7 +1325,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>34</v>
       </c>
@@ -1286,7 +1333,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>57</v>
       </c>
@@ -1294,7 +1341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>59</v>
       </c>
@@ -1302,7 +1349,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1322,7 +1369,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>34</v>
       </c>
@@ -1330,7 +1377,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>57</v>
       </c>
@@ -1338,7 +1385,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>59</v>
       </c>
@@ -1346,7 +1393,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1369,7 +1416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1386,7 +1433,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>70</v>
       </c>
@@ -1394,7 +1441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>72</v>
       </c>
@@ -1402,7 +1449,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>74</v>
       </c>
@@ -1410,7 +1457,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>76</v>
       </c>
@@ -1418,7 +1465,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>78</v>
       </c>
@@ -1426,7 +1473,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>80</v>
       </c>
@@ -1434,7 +1481,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>82</v>
       </c>
@@ -1442,7 +1489,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -1462,7 +1509,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -1482,7 +1529,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1502,7 +1549,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -1522,7 +1569,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>183</v>
       </c>
@@ -1533,7 +1580,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>185</v>
       </c>
@@ -1544,7 +1591,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -1561,7 +1608,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -1578,7 +1625,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -1598,7 +1645,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>99</v>
       </c>
@@ -1606,7 +1653,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>101</v>
       </c>
@@ -1614,7 +1661,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>104</v>
       </c>
@@ -1637,7 +1684,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -1663,7 +1710,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1680,7 +1727,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1697,315 +1744,339 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
       <c r="J41" t="s">
         <v>49</v>
       </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="F42" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" t="s">
-        <v>117</v>
-      </c>
-      <c r="I42" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
-      </c>
-      <c r="I43" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
-      <c r="A44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" t="s">
-        <v>23</v>
-      </c>
-      <c r="J44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>191</v>
+        <v>129</v>
       </c>
       <c r="J45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>130</v>
+      </c>
+      <c r="C46" t="s">
+        <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E46" t="s">
+        <v>129</v>
+      </c>
+      <c r="J46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" t="s">
         <v>19</v>
       </c>
-      <c r="J46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="F47" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="F48" t="s">
-        <v>126</v>
-      </c>
-      <c r="G48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="J48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" t="s">
         <v>129</v>
       </c>
       <c r="J49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" t="s">
-        <v>130</v>
-      </c>
-      <c r="C50" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50" t="s">
+        <v>46</v>
+      </c>
+      <c r="P49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>125</v>
+      </c>
+      <c r="G50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>126</v>
+      </c>
+      <c r="G51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" t="s">
+        <v>145</v>
+      </c>
+      <c r="J54" t="s">
+        <v>46</v>
+      </c>
+      <c r="P54" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>143</v>
+      </c>
+      <c r="G55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>145</v>
+      </c>
+      <c r="G56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" t="s">
         <v>129</v>
       </c>
-      <c r="J50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16">
-      <c r="A51" t="s">
-        <v>40</v>
-      </c>
-      <c r="B51" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" t="s">
-        <v>128</v>
-      </c>
-      <c r="D51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="J51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16">
-      <c r="A52" t="s">
-        <v>41</v>
-      </c>
-      <c r="B52" t="s">
-        <v>133</v>
-      </c>
-      <c r="C52" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" t="s">
-        <v>41</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16">
-      <c r="A53" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" t="s">
-        <v>134</v>
-      </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" t="s">
-        <v>129</v>
-      </c>
-      <c r="J53" t="s">
-        <v>46</v>
-      </c>
-      <c r="P53" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="F54" t="s">
-        <v>125</v>
-      </c>
-      <c r="G54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16">
-      <c r="F55" t="s">
-        <v>126</v>
-      </c>
-      <c r="G55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" t="s">
-        <v>137</v>
-      </c>
-      <c r="B56" t="s">
-        <v>138</v>
-      </c>
-      <c r="C56" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16">
-      <c r="A57" t="s">
-        <v>139</v>
-      </c>
-      <c r="B57" t="s">
-        <v>140</v>
-      </c>
-      <c r="C57" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="J57" t="s">
+        <v>49</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>149</v>
+      </c>
+      <c r="C58" t="s">
+        <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
-      <c r="I58" t="s">
-        <v>145</v>
-      </c>
       <c r="J58" t="s">
         <v>46</v>
       </c>
-      <c r="P58" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16">
-      <c r="F59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G59" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16">
-      <c r="F60" t="s">
-        <v>145</v>
-      </c>
-      <c r="G60" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16">
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60" t="s">
+        <v>46</v>
+      </c>
+      <c r="P60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" t="s">
         <v>148</v>
       </c>
-      <c r="B61" t="s">
-        <v>147</v>
-      </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>129</v>
+        <v>19</v>
       </c>
       <c r="J61" t="s">
-        <v>49</v>
-      </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
         <v>148</v>
@@ -2020,12 +2091,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C63" t="s">
         <v>148</v>
@@ -2040,12 +2111,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B64" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C64" t="s">
         <v>148</v>
@@ -2059,221 +2130,223 @@
       <c r="J64" t="s">
         <v>46</v>
       </c>
-      <c r="P64" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17">
-      <c r="A65" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" t="s">
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>164</v>
+      </c>
+      <c r="G65" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>168</v>
+      </c>
+      <c r="G67" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>170</v>
+      </c>
+      <c r="G68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>172</v>
+      </c>
+      <c r="G69" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>174</v>
+      </c>
+      <c r="G70" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" t="s">
         <v>148</v>
       </c>
-      <c r="D65" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
+        <v>191</v>
+      </c>
+      <c r="J71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>179</v>
+      </c>
+      <c r="B72" t="s">
+        <v>178</v>
+      </c>
+      <c r="C72" t="s">
+        <v>148</v>
+      </c>
+      <c r="D72" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" t="s">
         <v>19</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J72" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
-      <c r="A66" t="s">
-        <v>158</v>
-      </c>
-      <c r="B66" t="s">
-        <v>159</v>
-      </c>
-      <c r="C66" t="s">
-        <v>148</v>
-      </c>
-      <c r="D66" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" t="s">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" t="s">
+        <v>187</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
         <v>19</v>
       </c>
-      <c r="J66" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17">
-      <c r="A67" t="s">
-        <v>160</v>
-      </c>
-      <c r="B67" t="s">
-        <v>161</v>
-      </c>
-      <c r="C67" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" t="s">
-        <v>19</v>
-      </c>
-      <c r="J67" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17">
-      <c r="A68" t="s">
-        <v>163</v>
-      </c>
-      <c r="B68" t="s">
-        <v>162</v>
-      </c>
-      <c r="C68" t="s">
-        <v>148</v>
-      </c>
-      <c r="D68" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" t="s">
-        <v>19</v>
-      </c>
-      <c r="J68" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17">
-      <c r="F69" t="s">
-        <v>164</v>
-      </c>
-      <c r="G69" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17">
-      <c r="F70" t="s">
-        <v>166</v>
-      </c>
-      <c r="G70" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17">
-      <c r="F71" t="s">
-        <v>168</v>
-      </c>
-      <c r="G71" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17">
-      <c r="F72" t="s">
-        <v>170</v>
-      </c>
-      <c r="G72" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17">
-      <c r="F73" t="s">
-        <v>172</v>
-      </c>
-      <c r="G73" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17">
-      <c r="F74" t="s">
-        <v>174</v>
-      </c>
-      <c r="G74" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17">
+      <c r="J73" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" t="s">
+        <v>193</v>
+      </c>
+      <c r="D74" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" t="s">
+        <v>129</v>
+      </c>
+      <c r="J74" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="C75" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E75" t="s">
-        <v>191</v>
+        <v>23</v>
       </c>
       <c r="J75" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="76" spans="1:17">
-      <c r="A76" t="s">
-        <v>179</v>
-      </c>
-      <c r="B76" t="s">
-        <v>178</v>
-      </c>
-      <c r="C76" t="s">
-        <v>148</v>
-      </c>
-      <c r="D76" t="s">
-        <v>27</v>
-      </c>
-      <c r="E76" t="s">
-        <v>19</v>
-      </c>
-      <c r="J76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17">
-      <c r="A77" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" t="s">
-        <v>187</v>
-      </c>
-      <c r="D77" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" t="s">
-        <v>19</v>
-      </c>
-      <c r="J77" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2000" spans="4:4">
-      <c r="D2000" t="s">
+      <c r="K75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G76" t="s">
+        <v>117</v>
+      </c>
+      <c r="I76" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>118</v>
+      </c>
+      <c r="G77" t="s">
+        <v>119</v>
+      </c>
+      <c r="I77" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>38</v>
+      </c>
+      <c r="B78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78" t="s">
+        <v>192</v>
+      </c>
+      <c r="D78" t="s">
+        <v>38</v>
+      </c>
+      <c r="E78" t="s">
+        <v>23</v>
+      </c>
+      <c r="J78" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1996" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1996" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E32:E2000 E2:E29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E29 E32:E1996" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J29 J32:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J29 J32:J1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2001:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1997:E1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT(ADDRESS(ROW(), 4))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29 D32:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29 D32:D1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>FieldType</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E74" listDataValidation="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -2282,19 +2355,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="5" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>180</v>
       </c>
@@ -2302,7 +2376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -2313,7 +2387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>39</v>
       </c>
@@ -2329,7 +2403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -2337,7 +2411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -2345,7 +2419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -2353,7 +2427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -2361,7 +2435,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -2372,7 +2446,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -2380,73 +2454,78 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D1:D25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D25">
     <sortCondition ref="D1:D25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2454,12 +2533,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>